<commit_message>
renamed list names | databases
</commit_message>
<xml_diff>
--- a/2025/first_semester/usupova_n_m/databases/excel_tasks/autocomplete_and_links_7_20.xlsx
+++ b/2025/first_semester/usupova_n_m/databases/excel_tasks/autocomplete_and_links_7_20.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iskenderkanimetov/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iskenderkanimetov/Documents/univer-tasks/2025/first_semester/usupova_n_m/databases/excel_tasks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF1AF251-A4FA-EC4B-BF31-70C468EF188D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BAF277-B6D9-1A40-80C4-D1DAA1C34D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{36C1DF69-0363-0147-A092-61E5ECCCFA73}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ведомость" sheetId="1" r:id="rId1"/>
-    <sheet name="Ведомость(Диаграмма)" sheetId="2" r:id="rId2"/>
+    <sheet name="Относительные ссылки" sheetId="1" r:id="rId1"/>
+    <sheet name="Диаграмма 1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,7 +99,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;сом&quot;_-;\-* #,##0.00\ &quot;сом&quot;_-;_-* &quot;-&quot;??\ &quot;сом&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;сом&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;сом&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -202,23 +202,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -304,7 +304,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Ведомость!$B$4:$B$13</c:f>
+              <c:f>'Относительные ссылки'!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -342,7 +342,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ведомость!$E$4:$E$13</c:f>
+              <c:f>'Относительные ссылки'!$E$4:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>_("сом"* #,##0.00_);_("сом"* \(#,##0.00\);_("сом"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
@@ -400,7 +400,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Ведомость!$B$4:$B$13</c:f>
+              <c:f>'Относительные ссылки'!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -438,7 +438,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ведомость!$G$4:$G$13</c:f>
+              <c:f>'Относительные ссылки'!$G$4:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>_("сом"* #,##0.00_);_("сом"* \(#,##0.00\);_("сом"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
@@ -783,7 +783,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Ведомость!$B$4:$B$13</c:f>
+              <c:f>'Относительные ссылки'!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -821,7 +821,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ведомость!$E$4:$E$13</c:f>
+              <c:f>'Относительные ссылки'!$E$4:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>_("сом"* #,##0.00_);_("сом"* \(#,##0.00\);_("сом"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
@@ -882,7 +882,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Ведомость!$B$4:$B$13</c:f>
+              <c:f>'Относительные ссылки'!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -920,7 +920,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ведомость!$G$4:$G$13</c:f>
+              <c:f>'Относительные ссылки'!$G$4:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>_("сом"* #,##0.00_);_("сом"* \(#,##0.00\);_("сом"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2304,7 +2304,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6076882"/>
+    <xdr:ext cx="9305906" cy="6067778"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Диаграмма 1">
@@ -2666,24 +2666,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -2709,261 +2709,261 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>720</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>22</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <f t="shared" ref="E4:E13" si="0">C4*D4</f>
         <v>15840</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <f t="shared" ref="F4:F13" si="1">E4*13%</f>
         <v>2059.2000000000003</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <f>E4-F4</f>
         <v>13780.8</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>770</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>15</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <f t="shared" si="0"/>
         <v>11550</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <f t="shared" si="1"/>
         <v>1501.5</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f t="shared" ref="G5:G13" si="2">E5-F5</f>
         <v>10048.5</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>820</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>16</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
         <v>13120</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f t="shared" si="1"/>
         <v>1705.6000000000001</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <f t="shared" si="2"/>
         <v>11414.4</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>820</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>21</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <f t="shared" si="0"/>
         <v>17220</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f t="shared" si="1"/>
         <v>2238.6</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <f t="shared" si="2"/>
         <v>14981.4</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>770</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>20</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <f t="shared" si="0"/>
         <v>15400</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f t="shared" si="1"/>
         <v>2002</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <f t="shared" si="2"/>
         <v>13398</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>720</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>19</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f t="shared" si="0"/>
         <v>13680</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>1778.4</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f t="shared" si="2"/>
         <v>11901.6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>720</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>14</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <f t="shared" si="0"/>
         <v>10080</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <f t="shared" si="1"/>
         <v>1310.4000000000001</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <f t="shared" si="2"/>
         <v>8769.6</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>820</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>16</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <f t="shared" si="0"/>
         <v>13120</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <f t="shared" si="1"/>
         <v>1705.6000000000001</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <f t="shared" si="2"/>
         <v>11414.4</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>770</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>12</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <f t="shared" si="0"/>
         <v>9240</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <f t="shared" si="1"/>
         <v>1201.2</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <f t="shared" si="2"/>
         <v>8038.8</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>820</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>22</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <f t="shared" si="0"/>
         <v>18040</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <f t="shared" si="1"/>
         <v>2345.2000000000003</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <f t="shared" si="2"/>
         <v>15694.8</v>
       </c>

</xml_diff>